<commit_message>
just updating new bfds
</commit_message>
<xml_diff>
--- a/Env/Problem_basis/Solution_info.xlsx
+++ b/Env/Problem_basis/Solution_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Programming\AI, Ml, data\Chem Eng RL\DistillationTrain-Gym\Env\Problem_basis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A663D693-1258-4F6F-AD24-6C6E69C127F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E34FEE-A830-4B19-82EB-05481E955F9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B-T-x" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>TAC</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Solution Current 2</t>
+  </si>
+  <si>
+    <t>Column TAC</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -472,6 +475,7 @@
     <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -626,6 +630,12 @@
         <f t="shared" si="0"/>
         <v>5.2189851280757757</v>
       </c>
+      <c r="K11" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11">
+        <v>13.17</v>
+      </c>
     </row>
     <row r="12" spans="1:15">
       <c r="F12">
@@ -635,6 +645,12 @@
       <c r="G12" t="s">
         <v>25</v>
       </c>
+      <c r="K12" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12">
+        <v>0.45</v>
+      </c>
     </row>
     <row r="15" spans="1:15">
       <c r="F15" t="s">
@@ -647,6 +663,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fix BFD maker pressure units
</commit_message>
<xml_diff>
--- a/Env/Problem_basis/Solution_info.xlsx
+++ b/Env/Problem_basis/Solution_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Programming\AI, Ml, data\Chem Eng RL\DistillationTrain-Gym\Env\Problem_basis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E34FEE-A830-4B19-82EB-05481E955F9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3057CE01-6AE3-4D2F-8F1D-956DB4A6A38C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -465,7 +465,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>